<commit_message>
endpoint se zona do imovel aceita tipo empreendimento HIS/HMP
</commit_message>
<xml_diff>
--- a/data/dados_zoneamento_his.xlsx
+++ b/data/dados_zoneamento_his.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d835916\Desktop\SISTEMAS\geoBdt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D01FA5-54CF-4D5E-90F5-3B966DD88140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9968AF27-BC8E-4A9E-9DDF-842D24E8A1BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="taxa_permeab_min" sheetId="1" r:id="rId1"/>
     <sheet name="Padrão de ocupação por Zona " sheetId="2" r:id="rId2"/>
     <sheet name="padrao_ocup_HIS" sheetId="3" r:id="rId3"/>
-    <sheet name="categoria admitida pro zona" sheetId="4" r:id="rId4"/>
+    <sheet name="categoria_admitida_por_zona" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
   <si>
     <t>Perímetro de Qualificação Ambiental</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>tx_permeab_&gt;500</t>
+  </si>
+  <si>
+    <t>codigo_siszon</t>
+  </si>
+  <si>
+    <t>sigla_zona</t>
   </si>
 </sst>
 </file>
@@ -731,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,7 +918,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,7 +2041,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A2" sqref="A2:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2975,8 +2981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A27"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2992,7 +2998,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
       </c>
       <c r="C1" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
tratamento para quando o parâmetro maximo ou minimo é nulo
</commit_message>
<xml_diff>
--- a/data/dados_zoneamento_his.xlsx
+++ b/data/dados_zoneamento_his.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d835916\Desktop\SISTEMAS\geoBdt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9968AF27-BC8E-4A9E-9DDF-842D24E8A1BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE0E838-DA0B-4F70-AC12-5AC79DD8554C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="taxa_permeab_min" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t>Perímetro de Qualificação Ambiental</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>sigla_zona</t>
+  </si>
+  <si>
+    <t>Coeficiente de Aproveitamento mínimo</t>
+  </si>
+  <si>
+    <t>Coeficiente de Aproveitamento Máximo básico</t>
   </si>
 </sst>
 </file>
@@ -2040,8 +2046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:M27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,10 +2108,10 @@
         <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
         <v>90</v>
@@ -2981,7 +2987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>